<commit_message>
commit addd global repo
</commit_message>
<xml_diff>
--- a/STM2_ECU/HW/man_files/estimation_prix_ECU.xlsx
+++ b/STM2_ECU/HW/man_files/estimation_prix_ECU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\ECU_STM_V1\STM2_ECU\HW\man_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -371,98 +371,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:I17"/>
+  <dimension ref="C4:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>120</v>
-      </c>
-      <c r="I4">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5">
         <v>40</v>
       </c>
-      <c r="I5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>40</v>
-      </c>
-      <c r="I6">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="I7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
         <v>50</v>
       </c>
-      <c r="I8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
-      <c r="I9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="E11">
         <f>SUM(E4:E9)</f>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="E13">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>8</v>
       </c>
@@ -475,7 +457,7 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <v>790</v>
+        <v>795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>